<commit_message>
added files to prep for zipping for assignment hand in
</commit_message>
<xml_diff>
--- a/Work Breakdown Structure (Peer Review).xlsx
+++ b/Work Breakdown Structure (Peer Review).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\TA and tutors\briefing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyeyo\SC2002-Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DFEA9F-0F37-4332-9CAF-96E13A6E7389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C02C6E-4A07-4FD8-A438-EA9C9214617E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">                      Tasks                                 Team Member</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Issue Tracking</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>* Project Manager</t>
   </si>
   <si>
@@ -91,12 +88,6 @@
     <t>Demo</t>
   </si>
   <si>
-    <t>main.class</t>
-  </si>
-  <si>
-    <t>.class</t>
-  </si>
-  <si>
     <t>Overall individual contribution (by deafult, equal for every member)</t>
   </si>
   <si>
@@ -107,6 +98,24 @@
   </si>
   <si>
     <t>Sequence Diagram</t>
+  </si>
+  <si>
+    <t>Choo Kye Yong</t>
+  </si>
+  <si>
+    <t>KEVIN LIM ERN KEE</t>
+  </si>
+  <si>
+    <t>MISHRA ADITI RAKESH</t>
+  </si>
+  <si>
+    <t>RAASHI SINGH</t>
+  </si>
+  <si>
+    <t>TOM TANG GUAN LIANG</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -670,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CB27"/>
+  <dimension ref="A1:BW27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,14 +690,12 @@
     <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="17" max="17" width="36.21875" customWidth="1"/>
+    <col min="12" max="12" width="36.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:75" ht="57.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -696,7 +703,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:80" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:75" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -704,38 +711,38 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:80" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:75" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
     </row>
-    <row r="7" spans="1:80" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:75" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1</v>
@@ -744,24 +751,22 @@
         <v>2</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="L7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -820,60 +825,54 @@
       <c r="BU7" s="1"/>
       <c r="BV7" s="1"/>
       <c r="BW7" s="1"/>
-      <c r="BX7" s="1"/>
-      <c r="BY7" s="1"/>
-      <c r="BZ7" s="1"/>
-      <c r="CA7" s="1"/>
-      <c r="CB7" s="1"/>
-    </row>
-    <row r="8" spans="1:80" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4">
+        <v>100</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
+      <c r="L8" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4">
+        <v>100</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+      <c r="L9" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4">
+        <v>100</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -882,18 +881,17 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="L10" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="4">
+        <v>100</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -903,37 +901,33 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:80" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="L11" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:75" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="4">
+        <v>50</v>
+      </c>
+      <c r="E12" s="4">
+        <v>50</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:80" x14ac:dyDescent="0.3">
+      <c r="L12" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -945,14 +939,9 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="23"/>
-    </row>
-    <row r="14" spans="1:80" x14ac:dyDescent="0.3">
+      <c r="L13" s="23"/>
+    </row>
+    <row r="14" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -964,14 +953,9 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="23"/>
-    </row>
-    <row r="15" spans="1:80" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L14" s="23"/>
+    </row>
+    <row r="15" spans="1:75" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -983,67 +967,42 @@
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="24"/>
-    </row>
-    <row r="16" spans="1:80" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L15" s="24"/>
+    </row>
+    <row r="16" spans="1:75" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="14">
         <f>SUM(B8:B15)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14">
-        <f t="shared" ref="D16:L16" si="0">SUM(D8:D15)</f>
-        <v>0</v>
+        <f t="shared" ref="D16:G16" si="0">SUM(D8:D15)</f>
+        <v>50</v>
       </c>
       <c r="E16" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F16" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G16" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="25"/>
+        <v>100</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="25"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1051,39 +1010,39 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>